<commit_message>
change carIntensityFactorKey to carIntensityFactorFirstKey
</commit_message>
<xml_diff>
--- a/src/tests/closework-option.test-cases.xlsx
+++ b/src/tests/closework-option.test-cases.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/naoto/Documents/projects/code-for-japan/JibungotoPlanet-backend/src/tests/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5C6B36D6-A43C-9F45-BE11-0A20A535726D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BE3D02DD-5151-6A40-BC72-D3779A68C26B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="2920" yWindow="2340" windowWidth="31640" windowHeight="19760" xr2:uid="{504EB999-7D82-6E4A-B2A0-71B74C50F3FE}"/>
   </bookViews>
@@ -465,10 +465,6 @@
     <phoneticPr fontId="1"/>
   </si>
   <si>
-    <t>carIntensityFactorKey</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
     <t>carChargingKey</t>
     <phoneticPr fontId="1"/>
   </si>
@@ -526,10 +522,6 @@
   </si>
   <si>
     <t>motorbikeWeeklyTravelingTime</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>gasoline_driving-factor</t>
     <phoneticPr fontId="1"/>
   </si>
   <si>
@@ -819,6 +811,14 @@
   </si>
   <si>
     <t>hasTravelingTime</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>carIntensityFactorFirstKey</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>gasoline</t>
     <phoneticPr fontId="1"/>
   </si>
 </sst>
@@ -1281,15 +1281,6 @@
     <xf numFmtId="177" fontId="7" fillId="3" borderId="19" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="177" fontId="7" fillId="3" borderId="20" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="9" fillId="3" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
@@ -1309,6 +1300,15 @@
     </xf>
     <xf numFmtId="0" fontId="8" fillId="3" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="12" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="パーセント" xfId="1" builtinId="5"/>
@@ -2558,7 +2558,7 @@
   <dimension ref="A1:E18"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <selection activeCell="C12" sqref="C12"/>
+      <selection activeCell="C3" sqref="C3:D3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="20"/>
@@ -2587,7 +2587,7 @@
     </row>
     <row r="2" spans="1:5">
       <c r="A2" s="18" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="B2" s="18" t="s">
         <v>55</v>
@@ -2599,21 +2599,21 @@
         <v>1</v>
       </c>
       <c r="E2" s="18" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
     </row>
     <row r="3" spans="1:5">
       <c r="A3" s="1" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="B3" s="1" t="s">
         <v>54</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>57</v>
+        <v>118</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>73</v>
+        <v>119</v>
       </c>
       <c r="E3" s="1" t="s">
         <v>16</v>
@@ -2621,13 +2621,13 @@
     </row>
     <row r="4" spans="1:5">
       <c r="A4" s="1" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="B4" s="1" t="s">
         <v>54</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="D4" s="1" t="s">
         <v>52</v>
@@ -2638,16 +2638,16 @@
     </row>
     <row r="5" spans="1:5">
       <c r="A5" s="1" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="B5" s="1" t="s">
         <v>54</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="D5" s="1" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="E5" s="1" t="s">
         <v>16</v>
@@ -2655,13 +2655,13 @@
     </row>
     <row r="6" spans="1:5">
       <c r="A6" s="1" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="B6" s="1" t="s">
         <v>54</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="D6" s="1">
         <v>5000</v>
@@ -2672,13 +2672,13 @@
     </row>
     <row r="7" spans="1:5">
       <c r="A7" s="1" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="B7" s="1" t="s">
         <v>54</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="D7" s="1">
         <v>5</v>
@@ -2689,13 +2689,13 @@
     </row>
     <row r="8" spans="1:5">
       <c r="A8" s="1" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="B8" s="1" t="s">
         <v>54</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="D8" s="1">
         <v>1</v>
@@ -2706,13 +2706,13 @@
     </row>
     <row r="9" spans="1:5">
       <c r="A9" s="1" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="B9" s="1" t="s">
         <v>54</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="D9" s="1">
         <v>1</v>
@@ -2723,13 +2723,13 @@
     </row>
     <row r="10" spans="1:5">
       <c r="A10" s="1" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="B10" s="1" t="s">
         <v>54</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="D10" s="1">
         <v>1</v>
@@ -2740,30 +2740,30 @@
     </row>
     <row r="11" spans="1:5">
       <c r="A11" s="1" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="B11" s="1" t="s">
         <v>54</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
       <c r="D11" s="1" t="b">
         <v>1</v>
       </c>
       <c r="E11" s="1" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
     </row>
     <row r="12" spans="1:5">
       <c r="A12" s="1" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="B12" s="1" t="s">
         <v>54</v>
       </c>
       <c r="C12" s="1" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="D12" s="1" t="s">
         <v>52</v>
@@ -2774,13 +2774,13 @@
     </row>
     <row r="13" spans="1:5">
       <c r="A13" s="1" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="B13" s="1" t="s">
         <v>54</v>
       </c>
       <c r="C13" s="1" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="D13" s="1">
         <v>20</v>
@@ -2791,13 +2791,13 @@
     </row>
     <row r="14" spans="1:5">
       <c r="A14" s="1" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="B14" s="1" t="s">
         <v>54</v>
       </c>
       <c r="C14" s="1" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="D14" s="1">
         <v>20</v>
@@ -2808,13 +2808,13 @@
     </row>
     <row r="15" spans="1:5">
       <c r="A15" s="1" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="B15" s="1" t="s">
         <v>54</v>
       </c>
       <c r="C15" s="1" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="D15" s="1">
         <v>20</v>
@@ -2825,13 +2825,13 @@
     </row>
     <row r="16" spans="1:5">
       <c r="A16" s="1" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="B16" s="1" t="s">
         <v>54</v>
       </c>
       <c r="C16" s="1" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="D16" s="1">
         <v>2</v>
@@ -2842,13 +2842,13 @@
     </row>
     <row r="17" spans="1:5">
       <c r="A17" s="1" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="B17" s="1" t="s">
         <v>54</v>
       </c>
       <c r="C17" s="1" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="D17" s="1">
         <v>20</v>
@@ -2859,13 +2859,13 @@
     </row>
     <row r="18" spans="1:5">
       <c r="A18" s="2" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="B18" s="2" t="s">
         <v>54</v>
       </c>
       <c r="C18" s="2" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="D18" s="2">
         <v>3</v>
@@ -2943,21 +2943,21 @@
       <c r="K1" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="L1" s="31" t="s">
-        <v>103</v>
-      </c>
-      <c r="M1" s="32"/>
-      <c r="N1" s="33"/>
+      <c r="L1" s="42" t="s">
+        <v>101</v>
+      </c>
+      <c r="M1" s="43"/>
+      <c r="N1" s="44"/>
     </row>
     <row r="2" spans="1:14">
       <c r="A2" s="4" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="B2" s="4" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="C2" s="4" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="D2" s="27">
         <v>12000</v>
@@ -2983,26 +2983,26 @@
       <c r="K2" s="7" t="s">
         <v>23</v>
       </c>
-      <c r="L2" s="34" t="s">
-        <v>106</v>
-      </c>
-      <c r="M2" s="35">
+      <c r="L2" s="31" t="s">
+        <v>104</v>
+      </c>
+      <c r="M2" s="32">
         <v>0</v>
       </c>
-      <c r="N2" s="36">
+      <c r="N2" s="33">
         <f>M2*(1-$AJ$90)</f>
         <v>0</v>
       </c>
     </row>
     <row r="3" spans="1:14">
       <c r="A3" s="8" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="B3" s="8" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="C3" s="8" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="D3" s="29">
         <v>12871.86785907957</v>
@@ -3028,26 +3028,26 @@
       <c r="K3" s="7" t="s">
         <v>26</v>
       </c>
-      <c r="L3" s="37" t="s">
-        <v>107</v>
-      </c>
-      <c r="M3" s="38">
+      <c r="L3" s="34" t="s">
+        <v>105</v>
+      </c>
+      <c r="M3" s="35">
         <v>0.60363760305930902</v>
       </c>
-      <c r="N3" s="39">
+      <c r="N3" s="36">
         <f t="shared" ref="N3:N10" si="0">M3*(1-$AJ$90)</f>
         <v>0.60363760305930902</v>
       </c>
     </row>
     <row r="4" spans="1:14">
       <c r="A4" s="8" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="B4" s="8" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="C4" s="8" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="D4" s="29">
         <v>1400.1196480539465</v>
@@ -3073,26 +3073,26 @@
       <c r="K4" s="7" t="s">
         <v>28</v>
       </c>
-      <c r="L4" s="37" t="s">
-        <v>108</v>
-      </c>
-      <c r="M4" s="38">
+      <c r="L4" s="34" t="s">
+        <v>106</v>
+      </c>
+      <c r="M4" s="35">
         <v>0.15884894415521755</v>
       </c>
-      <c r="N4" s="39">
+      <c r="N4" s="36">
         <f t="shared" si="0"/>
         <v>0.15884894415521755</v>
       </c>
     </row>
     <row r="5" spans="1:14">
       <c r="A5" s="8" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="B5" s="8" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="C5" s="8" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="D5" s="29">
         <v>120</v>
@@ -3118,26 +3118,26 @@
       <c r="K5" s="7" t="s">
         <v>30</v>
       </c>
-      <c r="L5" s="37" t="s">
-        <v>109</v>
-      </c>
-      <c r="M5" s="38">
+      <c r="L5" s="34" t="s">
+        <v>107</v>
+      </c>
+      <c r="M5" s="35">
         <v>0</v>
       </c>
-      <c r="N5" s="39">
+      <c r="N5" s="36">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
     <row r="6" spans="1:14">
       <c r="A6" s="8" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="B6" s="8" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="C6" s="8" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="D6" s="29">
         <v>1029.7037173899421</v>
@@ -3163,26 +3163,26 @@
       <c r="K6" s="7" t="s">
         <v>32</v>
       </c>
-      <c r="L6" s="37" t="s">
-        <v>110</v>
-      </c>
-      <c r="M6" s="38">
+      <c r="L6" s="34" t="s">
+        <v>108</v>
+      </c>
+      <c r="M6" s="35">
         <v>0.10410685214096388</v>
       </c>
-      <c r="N6" s="39">
+      <c r="N6" s="36">
         <f t="shared" si="0"/>
         <v>0.10410685214096388</v>
       </c>
     </row>
     <row r="7" spans="1:14">
       <c r="A7" s="8" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="B7" s="8" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="C7" s="8" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="D7" s="29">
         <v>4571.6765559219184</v>
@@ -3208,26 +3208,26 @@
       <c r="K7" s="7" t="s">
         <v>35</v>
       </c>
-      <c r="L7" s="37" t="s">
-        <v>111</v>
-      </c>
-      <c r="M7" s="38">
+      <c r="L7" s="34" t="s">
+        <v>109</v>
+      </c>
+      <c r="M7" s="35">
         <v>0.22558368054778968</v>
       </c>
-      <c r="N7" s="39">
+      <c r="N7" s="36">
         <f t="shared" si="0"/>
         <v>0.22558368054778968</v>
       </c>
     </row>
     <row r="8" spans="1:14">
       <c r="A8" s="8" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="B8" s="8" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="C8" s="8" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="D8" s="29">
         <v>1352.9120938264666</v>
@@ -3253,26 +3253,26 @@
       <c r="K8" s="7" t="s">
         <v>37</v>
       </c>
-      <c r="L8" s="37" t="s">
-        <v>112</v>
-      </c>
-      <c r="M8" s="38">
+      <c r="L8" s="34" t="s">
+        <v>110</v>
+      </c>
+      <c r="M8" s="35">
         <v>0</v>
       </c>
-      <c r="N8" s="39">
+      <c r="N8" s="36">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
     <row r="9" spans="1:14">
       <c r="A9" s="8" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="B9" s="8" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="C9" s="8" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="D9" s="29">
         <v>1122.3905574331159</v>
@@ -3298,26 +3298,26 @@
       <c r="K9" s="7" t="s">
         <v>39</v>
       </c>
-      <c r="L9" s="37" t="s">
-        <v>113</v>
-      </c>
-      <c r="M9" s="38">
+      <c r="L9" s="34" t="s">
+        <v>111</v>
+      </c>
+      <c r="M9" s="35">
         <v>0.43584004864396131</v>
       </c>
-      <c r="N9" s="39">
+      <c r="N9" s="36">
         <f t="shared" si="0"/>
         <v>0.43584004864396131</v>
       </c>
     </row>
     <row r="10" spans="1:14" ht="21" thickBot="1">
       <c r="A10" s="8" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="B10" s="8" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="C10" s="8" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="D10" s="28">
         <v>211.06470120834891</v>
@@ -3343,26 +3343,26 @@
       <c r="K10" s="7" t="s">
         <v>42</v>
       </c>
-      <c r="L10" s="37" t="s">
-        <v>114</v>
-      </c>
-      <c r="M10" s="38">
+      <c r="L10" s="34" t="s">
+        <v>112</v>
+      </c>
+      <c r="M10" s="35">
         <v>0.52812257839178267</v>
       </c>
-      <c r="N10" s="39">
+      <c r="N10" s="36">
         <f t="shared" si="0"/>
         <v>0.52812257839178267</v>
       </c>
     </row>
     <row r="11" spans="1:14" ht="21" thickBot="1">
       <c r="A11" s="8" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="B11" s="8" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="C11" s="8" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="D11" s="26">
         <v>168.93444059755035</v>
@@ -3388,27 +3388,27 @@
       <c r="K11" s="7" t="s">
         <v>44</v>
       </c>
-      <c r="L11" s="40"/>
+      <c r="L11" s="37"/>
       <c r="M11" s="19"/>
-      <c r="N11" s="41" t="s">
-        <v>115</v>
+      <c r="N11" s="38" t="s">
+        <v>113</v>
       </c>
     </row>
     <row r="12" spans="1:14">
       <c r="A12" s="8" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="B12" s="8" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="C12" s="8" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="D12" s="27">
         <v>4.5814463195414844E-2</v>
       </c>
       <c r="E12" s="8" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="F12" s="8" t="s">
         <v>18</v>
@@ -3434,19 +3434,19 @@
     </row>
     <row r="13" spans="1:14">
       <c r="A13" s="8" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="B13" s="8" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="C13" s="8" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="D13" s="29">
         <v>1.1624128551545493E-2</v>
       </c>
       <c r="E13" s="8" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="F13" s="8" t="s">
         <v>18</v>
@@ -3466,29 +3466,29 @@
       <c r="K13" s="7" t="s">
         <v>46</v>
       </c>
-      <c r="L13" s="42" t="s">
-        <v>116</v>
-      </c>
-      <c r="M13" s="38">
+      <c r="L13" s="39" t="s">
+        <v>114</v>
+      </c>
+      <c r="M13" s="35">
         <v>0.620253164556962</v>
       </c>
-      <c r="N13" s="43"/>
+      <c r="N13" s="40"/>
     </row>
     <row r="14" spans="1:14">
       <c r="A14" s="8" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="B14" s="8" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="C14" s="8" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="D14" s="29">
         <v>3.5897022020564959</v>
       </c>
       <c r="E14" s="8" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="F14" s="8" t="s">
         <v>18</v>
@@ -3509,20 +3509,20 @@
         <v>48</v>
       </c>
       <c r="L14" s="21"/>
-      <c r="M14" s="44" t="s">
-        <v>117</v>
+      <c r="M14" s="41" t="s">
+        <v>115</v>
       </c>
       <c r="N14" s="20"/>
     </row>
     <row r="15" spans="1:14">
       <c r="A15" s="8" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="B15" s="8" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="C15" s="8" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="D15" s="29">
         <v>58.679038639035518</v>
@@ -3550,19 +3550,19 @@
       </c>
       <c r="L15" s="21"/>
       <c r="M15" s="19" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
       <c r="N15" s="20"/>
     </row>
     <row r="16" spans="1:14">
       <c r="A16" s="8" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="B16" s="8" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="C16" s="8" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="D16" s="29">
         <v>1.9677934088826179</v>
@@ -3594,13 +3594,13 @@
     </row>
     <row r="17" spans="1:14" ht="21" thickBot="1">
       <c r="A17" s="10" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="B17" s="10" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="C17" s="10" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="D17" s="28">
         <v>0.32510936147529401</v>

</xml_diff>